<commit_message>
Word footer & header, short hand for block, Excel sheet name checks
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_demo_140-xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_demo_140-xlsx.w3mi.data.xlsx
@@ -88,7 +88,7 @@
     <t>{R-BL_2020}</t>
   </si>
   <si>
-    <t>{R-BL3;type=block;cond=strlen( value-TITLE ) eq -1}</t>
+    <t>{R-BL3;=strlen( v-TITLE ) eq -1}</t>
   </si>
   <si>
     <r>
@@ -109,7 +109,7 @@
     </r>
   </si>
   <si>
-    <t>{R-BL2;type=block;cond=strlen( value-TITLE ) gt 0}</t>
+    <t>{R-BL2;=strlen( v-TITLE ) gt 0}</t>
   </si>
   <si>
     <t>Hide BL3</t>

</xml_diff>

<commit_message>
DEV warnings for Excel
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_demo_140-xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_demo_140-xlsx.w3mi.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\moldab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7833450-F01E-44E6-BAB1-3C6F30CCBCF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8ECADE-8345-4AA2-9D52-E6754C494144}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DD9765B2-999D-488B-95F5-A558A73EE175}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t xml:space="preserve">42.500 </t>
   </si>
   <si>
-    <t>{R-BL_2020}</t>
-  </si>
-  <si>
     <t>{R-BL3;=strlen( v-TITLE ) eq -1}</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>Delete 2 rows!</t>
+  </si>
+  <si>
+    <t>{R-BL_2020;comeeent=End of block}</t>
   </si>
 </sst>
 </file>
@@ -337,7 +337,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -353,9 +353,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,7 +393,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -499,7 +499,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -651,9 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAE5BAA-5943-423A-91C9-46DCD0649A5F}">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -682,7 +680,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -719,27 +717,27 @@
     </row>
     <row r="12" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="10"/>
     </row>

</xml_diff>